<commit_message>
added I'm batman, my precious
</commit_message>
<xml_diff>
--- a/SheldonMix/SheldonMix.Web/SheldonMix/Sounds.xlsx
+++ b/SheldonMix/SheldonMix.Web/SheldonMix/Sounds.xlsx
@@ -5,16 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucaspol\Source\Workspaces\WPaolo7\SheldonMix\SheldonMix.Web\SheldonMix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Luca\Documents\Visual Studio 2010\Projects\WPaolo7\SheldonMix\SheldonMix.Web\SheldonMix\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8148"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="5" r:id="rId3"/>
+  </pivotCaches>
 </workbook>
 </file>
 
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="128">
   <si>
     <t>Name</t>
   </si>
@@ -143,9 +147,6 @@
     <t>CLAS</t>
   </si>
   <si>
-    <t>oouh</t>
-  </si>
-  <si>
     <t>A plus !</t>
   </si>
   <si>
@@ -197,9 +198,6 @@
     <t>Toc toc toc Penny</t>
   </si>
   <si>
-    <t>mua ah ah</t>
-  </si>
-  <si>
     <t>peace out</t>
   </si>
   <si>
@@ -390,6 +388,33 @@
   </si>
   <si>
     <t>Doux_chaton_adorable_chaton.mp3</t>
+  </si>
+  <si>
+    <t>My precious</t>
+  </si>
+  <si>
+    <t>en_precious.mp3</t>
+  </si>
+  <si>
+    <t>I'm Batman</t>
+  </si>
+  <si>
+    <t>en_Im_Batman.mp3</t>
+  </si>
+  <si>
+    <t>Ooohu</t>
+  </si>
+  <si>
+    <t>Mua ah ah</t>
+  </si>
+  <si>
+    <t>Etichette di riga</t>
+  </si>
+  <si>
+    <t>Totale complessivo</t>
+  </si>
+  <si>
+    <t>Conteggio di Category</t>
   </si>
 </sst>
 </file>
@@ -425,12 +450,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -471,11 +501,1341 @@
 </MapInfo>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Sounds.xlsx]Foglio2!Tabella_pivot1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio2!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Totale</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Foglio2!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CLAS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>TBBT</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ZAZZ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio2!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Luca Spolidoro" refreshedDate="41860.682693634262" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="60">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Tabella1"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Name" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="File" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Category" numFmtId="0">
+      <sharedItems count="3">
+        <s v="CLAS"/>
+        <s v="TBBT"/>
+        <s v="ZAZZ"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Lang" numFmtId="0">
+      <sharedItems count="2">
+        <s v="fr-FR"/>
+        <s v="en-US"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="60">
+  <r>
+    <s v="Ce n'est pas grave, c'est horrible !"/>
+    <s v="Ce_n'est_pas_grave_c'est_horrible.mp3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Cela ne se passe jamais à merveille"/>
+    <s v="Cela_ne_se_passe_jamais_a_merveille.mp3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="C'est un mensonge"/>
+    <s v="C'est_un_mensonge.mp3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Doux chaton, adorable chaton"/>
+    <s v="Doux_chaton_adorable_chaton.mp3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="La chanson de Sheldon bourré"/>
+    <s v="La_chanson_de_Sheldon_bourre.mp3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Les oompa loompas de la science"/>
+    <s v="Les_oompa_loompas_de_la_science.mp3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Penny et Sheldon chantent"/>
+    <s v="Penny_et_Sheldon_chantent.mp3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Toc toc toc Penny"/>
+    <s v="Toc_toc_toc_Penny.mp3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Tu es à ma place"/>
+    <s v="Tu_es_a_ma_place.mp3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Tu m'auras pas"/>
+    <s v="Tu_m'auras_pas.mp3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Theme end"/>
+    <s v="TBBT_Theme_end.mp3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Theme full"/>
+    <s v="TBBT_Theme_full.mp3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="A plus !"/>
+    <s v="A_plus.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Bonjour mes petites céréales"/>
+    <s v="Bonjour_mes_petites_cereales.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Brave Léonard"/>
+    <s v="Brave_Leonard.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="C'est génial d'y aller en train"/>
+    <s v="C'est_genial_d'y_aller_en_train.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="C'est un piège !"/>
+    <s v="C'est_un_piege.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Dr Sheldon Cooper"/>
+    <s v="Dr_Sheldon_Cooper.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Je plaisantais"/>
+    <s v="Je_plaisantais.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Je possède l'ADN de Léonard Nimoy"/>
+    <s v="Je_possede_l'ADN_de_Leonard_Nimoy.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Je souhaite à Sheldon, une vie longue et prospère"/>
+    <s v="Je_souhaite_a_Sheldon_une_vie_longue_et_prospere.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Je vous salue mes amis"/>
+    <s v="Je_vous_salue_mes_amis.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="La la"/>
+    <s v="La_la.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Le compte WOW de Sheldon"/>
+    <s v="Le_compte_WOW_de_Sheldon.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Le rire de Sheldon"/>
+    <s v="Le_rire_de_Sheldon.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Mouahahahah"/>
+    <s v="Mouahahahah.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Pierre papier ciseaux lézard spock"/>
+    <s v="Pierre_papier_ciseaux_lezard_spock.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Sheldon est là"/>
+    <s v="Sheldon_est_la.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Sheldon raconte son rêve avec Spoke"/>
+    <s v="Sheldon_raconte_son_reve_avec_Spoke.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Whip eh hee"/>
+    <s v="Whip_eh_hee.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Bazinga one of my jokes"/>
+    <s v="CLAS_bazinga_one_of_my_jokes.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Bazinga!"/>
+    <s v="CLAS_Bazinga1.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Change is never fine"/>
+    <s v="CLAS_change_is_never_fine.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Hello honeypuffs"/>
+    <s v="CLAS_hello_honeypuffs.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="I'm Batman"/>
+    <s v="en_Im_Batman.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="It's not bad it's horrible"/>
+    <s v="CLAS_not_bad_it_s_horrible.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Knock knock knock Penny"/>
+    <s v="CLAS_knock_knock_knock_Penny.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Mua ah ah"/>
+    <s v="CLAS_mua_ah_ah.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Ooohu"/>
+    <s v="CLAS_oouh.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="peace out"/>
+    <s v="CLAS_peace_out.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Rock Paper Scissor Lizard Spock"/>
+    <s v="CLAS_Rock_Paper_Scissor_Lizard_Spock.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Sheldon laugh"/>
+    <s v="CLAS_Sheldon_laugh.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="there there"/>
+    <s v="CLAS_there_there.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="You're in my spot"/>
+    <s v="CLAS_You're_in_my_spot.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Theme end"/>
+    <s v="TBBT_Theme_end.mp3"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Theme full"/>
+    <s v="TBBT_Theme_full.mp3"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Bongo Song"/>
+    <s v="ZAZZ_Bongo_Song.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Brave Leonard song"/>
+    <s v="ZAZZ_Brave_Leonard_song.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="DNA of leonard nimoy"/>
+    <s v="ZAZZ_DNA_of_leonard_nimoy.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Dr Sheldon Cooper FTW"/>
+    <s v="ZAZZ_Dr_Sheldon_Cooper_FTW.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Engineering oompa loompas"/>
+    <s v="ZAZZ_Engineering_oompa_loompas.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="It's a trap!"/>
+    <s v="ZAZZ_It's_a_trap1.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="My precious"/>
+    <s v="en_precious.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Penny Blossom Song"/>
+    <s v="ZAZZ_Penny_Blossom_Song.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Sheldon sings drunk"/>
+    <s v="ZAZZ_Sheldon_drunk_sings.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Soft Kitty"/>
+    <s v="ZAZZ_Sheldon_soft_kitty.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="To Sheldon live long and prosper"/>
+    <s v="ZAZZ_To_Sheldon_live_long_and_prosper.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="we're taking the train"/>
+    <s v="ZAZZ_we're_taking_the_train.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Whip eh-hee"/>
+    <s v="ZAZZ_Whip_eh-hee.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="WoW Hacking"/>
+    <s v="ZAZZ_WoW_Hacking.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="3" item="0" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Conteggio di Category" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:D59" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:D59"/>
-  <sortState ref="A2:D59">
-    <sortCondition descending="1" ref="D1:D59"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:D61" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:D61"/>
+  <sortState ref="A2:D61">
+    <sortCondition descending="1" ref="D2:D61"/>
+    <sortCondition ref="C2:C61"/>
+    <sortCondition ref="A2:A61"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" uniqueName="Name" name="Name">
@@ -758,21 +2118,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.44140625" customWidth="1"/>
+    <col min="1" max="1" width="46.42578125" customWidth="1"/>
     <col min="2" max="2" width="57" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -786,68 +2146,68 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
+      <c r="C4" t="s">
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>118</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -856,26 +2216,26 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C8" t="s">
         <v>37</v>
@@ -884,12 +2244,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
@@ -898,12 +2258,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
@@ -912,124 +2272,124 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" t="s">
-        <v>119</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C15" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C18" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -1038,26 +2398,26 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -1066,26 +2426,26 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -1094,12 +2454,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -1108,12 +2468,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1122,54 +2482,54 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -1178,37 +2538,37 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
@@ -1220,9 +2580,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -1234,96 +2594,96 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>121</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
       <c r="C36" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>37</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>124</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>37</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
         <v>37</v>
@@ -1332,26 +2692,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>37</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
         <v>37</v>
@@ -1360,12 +2720,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
         <v>37</v>
@@ -1374,12 +2734,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C44" t="s">
         <v>37</v>
@@ -1388,12 +2748,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C45" t="s">
         <v>37</v>
@@ -1402,68 +2762,68 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="C47" t="s">
+        <v>36</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" t="s">
-        <v>37</v>
+        <v>23</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>4</v>
@@ -1472,12 +2832,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>4</v>
@@ -1486,54 +2846,54 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B52" t="s">
-        <v>21</v>
-      </c>
-      <c r="C52" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>120</v>
       </c>
       <c r="C54" t="s">
-        <v>37</v>
-      </c>
-      <c r="D54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>4</v>
@@ -1542,12 +2902,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>4</v>
@@ -1556,12 +2916,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B57" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>4</v>
@@ -1570,12 +2930,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>4</v>
@@ -1584,17 +2944,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>18</v>
-      </c>
-      <c r="C59" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D59" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1604,4 +2992,72 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="4">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added goodnight puny human
</commit_message>
<xml_diff>
--- a/SheldonMix/SheldonMix.Web/SheldonMix/Sounds.xlsx
+++ b/SheldonMix/SheldonMix.Web/SheldonMix/Sounds.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="130">
   <si>
     <t>Name</t>
   </si>
@@ -411,10 +411,16 @@
     <t>Etichette di riga</t>
   </si>
   <si>
-    <t>Totale complessivo</t>
-  </si>
-  <si>
     <t>Conteggio di Category</t>
+  </si>
+  <si>
+    <t>en_goodnight_puny_human.mp3</t>
+  </si>
+  <si>
+    <t>Goodnight puny human</t>
+  </si>
+  <si>
+    <t>Conteggio di Lang</t>
   </si>
 </sst>
 </file>
@@ -569,6 +575,48 @@
           <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -635,7 +683,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Foglio2!$A$4:$A$7</c:f>
+              <c:f>Foglio2!$A$4:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -652,7 +700,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio2!$B$4:$B$7</c:f>
+              <c:f>Foglio2!$B$4:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1762,8 +1810,49 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A10:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Conteggio di Lang" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1786,7 +1875,7 @@
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="4">
+  <rowItems count="3">
     <i>
       <x/>
     </i>
@@ -1795,9 +1884,6 @@
     </i>
     <i>
       <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
     </i>
   </rowItems>
   <colItems count="1">
@@ -1809,12 +1895,48 @@
   <dataFields count="1">
     <dataField name="Conteggio di Category" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="4">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -1830,12 +1952,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:D61" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:D61"/>
-  <sortState ref="A2:D61">
-    <sortCondition descending="1" ref="D2:D61"/>
-    <sortCondition ref="C2:C61"/>
-    <sortCondition ref="A2:A61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:D62" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:D62"/>
+  <sortState ref="A2:D62">
+    <sortCondition descending="1" ref="D2:D62"/>
+    <sortCondition ref="C2:C62"/>
+    <sortCondition ref="A2:A62"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" uniqueName="Name" name="Name">
@@ -2118,10 +2240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2862,10 +2984,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>128</v>
       </c>
       <c r="B53" t="s">
-        <v>27</v>
+        <v>127</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>4</v>
@@ -2876,38 +2998,38 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>73</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
-      </c>
-      <c r="C54" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="B55" t="s">
-        <v>28</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>4</v>
@@ -2918,10 +3040,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B57" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>4</v>
@@ -2932,10 +3054,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>4</v>
@@ -2946,10 +3068,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>4</v>
@@ -2960,10 +3082,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>4</v>
@@ -2974,15 +3096,29 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" t="s">
+        <v>33</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>71</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>34</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" s="1" t="s">
+      <c r="C62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2996,16 +3132,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3021,7 +3157,7 @@
         <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3048,16 +3184,32 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" s="4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="4">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix reload list automatically after liveupdate
</commit_message>
<xml_diff>
--- a/SheldonMix/SheldonMix.Web/SheldonMix/Sounds.xlsx
+++ b/SheldonMix/SheldonMix.Web/SheldonMix/Sounds.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="136">
   <si>
     <t>Name</t>
   </si>
@@ -427,6 +427,18 @@
   </si>
   <si>
     <t>Whip! Eh-hee</t>
+  </si>
+  <si>
+    <t>suffer_in_silence.mp3</t>
+  </si>
+  <si>
+    <t>Suffer in silence</t>
+  </si>
+  <si>
+    <t>When_Sheldon_Cries.mp3</t>
+  </si>
+  <si>
+    <t>When Sheldon cries</t>
   </si>
 </sst>
 </file>
@@ -532,7 +544,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -717,7 +728,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -744,7 +755,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1385,16 +1395,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1417,7 +1427,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Luca Spolidoro" refreshedDate="41867.478475578704" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="63">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Luca Spolidoro" refreshedDate="41867.507796759259" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabella1"/>
   </cacheSource>
@@ -1451,7 +1461,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="63">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="64">
   <r>
     <s v="Ce n'est pas grave, c'est horrible !"/>
     <s v="Ce_n'est_pas_grave_c'est_horrible.mp3"/>
@@ -1633,7 +1643,7 @@
     <x v="0"/>
   </r>
   <r>
-    <s v="Whip eh hee"/>
+    <s v="Whip! Eh-hee"/>
     <s v="Whip_eh_hee.mp3"/>
     <x v="2"/>
     <x v="0"/>
@@ -1711,7 +1721,7 @@
     <x v="1"/>
   </r>
   <r>
-    <s v="there there"/>
+    <s v="There there"/>
     <s v="CLAS_there_there.mp3"/>
     <x v="0"/>
     <x v="1"/>
@@ -1827,6 +1837,12 @@
   <r>
     <s v="WoW Hacking"/>
     <s v="ZAZZ_WoW_Hacking.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Suffer in silence"/>
+    <s v="suffer_in_silence.mp3"/>
     <x v="2"/>
     <x v="1"/>
   </r>
@@ -1834,7 +1850,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A10:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -1875,7 +1891,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -1976,12 +1992,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:D64" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:D64"/>
-  <sortState ref="A2:D64">
-    <sortCondition descending="1" ref="D2:D64"/>
-    <sortCondition ref="C2:C64"/>
-    <sortCondition ref="A2:A64"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:D66" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:D66"/>
+  <sortState ref="A2:D66">
+    <sortCondition descending="1" ref="D2:D66"/>
+    <sortCondition ref="C2:C66"/>
+    <sortCondition ref="A2:A66"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" uniqueName="Name" name="Name">
@@ -2264,10 +2280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,10 +2450,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
         <v>36</v>
@@ -2448,10 +2464,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
         <v>36</v>
@@ -2924,10 +2940,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C47" t="s">
         <v>36</v>
@@ -2938,10 +2954,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C48" t="s">
         <v>36</v>
@@ -3106,24 +3122,24 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>133</v>
       </c>
       <c r="B60" t="s">
-        <v>31</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D60" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>4</v>
@@ -3134,43 +3150,71 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>129</v>
+        <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>128</v>
-      </c>
-      <c r="C62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>129</v>
       </c>
       <c r="B63" t="s">
-        <v>33</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D63" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>135</v>
+      </c>
+      <c r="B64" t="s">
+        <v>134</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>70</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B66" t="s">
         <v>34</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D64" s="1" t="s">
+      <c r="C66" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3233,7 +3277,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3249,7 +3293,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new sound my brain is better
</commit_message>
<xml_diff>
--- a/SheldonMix/SheldonMix.Web/SheldonMix/Sounds.xlsx
+++ b/SheldonMix/SheldonMix.Web/SheldonMix/Sounds.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8150"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
-    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
+    <sheet name="Statistic" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="140">
   <si>
     <t>Name</t>
   </si>
@@ -402,9 +402,6 @@
     <t>Mua ah ah</t>
   </si>
   <si>
-    <t>Etichette di riga</t>
-  </si>
-  <si>
     <t>Conteggio di Category</t>
   </si>
   <si>
@@ -445,6 +442,15 @@
   </si>
   <si>
     <t>forgot_flash_drive.mp3</t>
+  </si>
+  <si>
+    <t>brain_better_than_everybody.mp3</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>My brain is better…</t>
   </si>
 </sst>
 </file>
@@ -490,7 +496,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -534,7 +540,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -545,12 +551,11 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Sounds.xlsx]Foglio2!Tabella_pivot1</c:name>
+    <c:name>[Sounds.xlsx]Statistic!Tabella_pivot1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -651,11 +656,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio2!$B$3</c:f>
+              <c:f>Statistic!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Totale</c:v>
+                  <c:v>Total</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -707,7 +712,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Foglio2!$A$4:$A$6</c:f>
+              <c:f>Statistic!$A$4:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -724,7 +729,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio2!$B$4:$B$6</c:f>
+              <c:f>Statistic!$B$4:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -735,7 +740,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -762,7 +767,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1435,7 +1439,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Luca Spolidoro" refreshedDate="41935.81619513889" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="66">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Luca Spolidoro" refreshedDate="42324.362512268519" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="67">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabella1"/>
   </cacheSource>
@@ -1469,7 +1473,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="66">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="67">
   <r>
     <s v="Ce n'est pas grave, c'est horrible !"/>
     <s v="Ce_n'est_pas_grave_c'est_horrible.mp3"/>
@@ -1531,315 +1535,327 @@
     <x v="0"/>
   </r>
   <r>
+    <s v="Theme end"/>
+    <s v="TBBT_Theme_end.mp3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
     <s v="Theme full"/>
     <s v="TBBT_Theme_full.mp3"/>
     <x v="1"/>
     <x v="0"/>
   </r>
   <r>
+    <s v="A plus !"/>
+    <s v="A_plus.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Bonjour mes petites céréales"/>
+    <s v="Bonjour_mes_petites_cereales.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Brave Léonard"/>
+    <s v="Brave_Leonard.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="C'est génial d'y aller en train"/>
+    <s v="C'est_genial_d'y_aller_en_train.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="C'est un piège !"/>
+    <s v="C'est_un_piege.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Dr Sheldon Cooper"/>
+    <s v="Dr_Sheldon_Cooper.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Je plaisantais"/>
+    <s v="Je_plaisantais.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Je possède l'ADN de Léonard Nimoy"/>
+    <s v="Je_possede_l'ADN_de_Leonard_Nimoy.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Je souhaite à Sheldon, une vie longue et prospère"/>
+    <s v="Je_souhaite_a_Sheldon_une_vie_longue_et_prospere.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Je vous salue mes amis"/>
+    <s v="Je_vous_salue_mes_amis.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="La la"/>
+    <s v="La_la.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Le compte WOW de Sheldon"/>
+    <s v="Le_compte_WOW_de_Sheldon.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Le rire de Sheldon"/>
+    <s v="Le_rire_de_Sheldon.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Mouahahahah"/>
+    <s v="Mouahahahah.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Pierre papier ciseaux lézard spock"/>
+    <s v="Pierre_papier_ciseaux_lezard_spock.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Sheldon est là"/>
+    <s v="Sheldon_est_la.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Sheldon raconte son rêve avec Spoke"/>
+    <s v="Sheldon_raconte_son_reve_avec_Spoke.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Wheaton Wheaton Wheaton!"/>
+    <s v="wheaton.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Whip! Eh-hee"/>
+    <s v="Whip_eh_hee.mp3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Bazinga one of my jokes"/>
+    <s v="CLAS_bazinga_one_of_my_jokes.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Bazinga!"/>
+    <s v="CLAS_Bazinga1.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Change is never fine"/>
+    <s v="CLAS_change_is_never_fine.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Hello honeypuffs"/>
+    <s v="CLAS_hello_honeypuffs.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="I'm Batman"/>
+    <s v="en_Im_Batman.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="It's not bad it's horrible"/>
+    <s v="CLAS_not_bad_it_s_horrible.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Knock knock knock Penny"/>
+    <s v="CLAS_knock_knock_knock_Penny.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Mua ah ah"/>
+    <s v="CLAS_mua_ah_ah.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Ooohu"/>
+    <s v="CLAS_oouh.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="peace out"/>
+    <s v="CLAS_peace_out.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Rock Paper Scissor Lizard Spock"/>
+    <s v="CLAS_Rock_Paper_Scissor_Lizard_Spock.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Sheldon laugh"/>
+    <s v="CLAS_Sheldon_laugh.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="There there"/>
+    <s v="CLAS_there_there.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="You're in my spot"/>
+    <s v="CLAS_You're_in_my_spot.mp3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
     <s v="Theme end"/>
     <s v="TBBT_Theme_end.mp3"/>
     <x v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="A plus !"/>
-    <s v="A_plus.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Bonjour mes petites céréales"/>
-    <s v="Bonjour_mes_petites_cereales.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Brave Léonard"/>
-    <s v="Brave_Leonard.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="C'est génial d'y aller en train"/>
-    <s v="C'est_genial_d'y_aller_en_train.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="C'est un piège !"/>
-    <s v="C'est_un_piege.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Dr Sheldon Cooper"/>
-    <s v="Dr_Sheldon_Cooper.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Je plaisantais"/>
-    <s v="Je_plaisantais.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Je possède l'ADN de Léonard Nimoy"/>
-    <s v="Je_possede_l'ADN_de_Leonard_Nimoy.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Je souhaite à Sheldon, une vie longue et prospère"/>
-    <s v="Je_souhaite_a_Sheldon_une_vie_longue_et_prospere.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Je vous salue mes amis"/>
-    <s v="Je_vous_salue_mes_amis.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="La la"/>
-    <s v="La_la.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Le compte WOW de Sheldon"/>
-    <s v="Le_compte_WOW_de_Sheldon.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Le rire de Sheldon"/>
-    <s v="Le_rire_de_Sheldon.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Mouahahahah"/>
-    <s v="Mouahahahah.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Pierre papier ciseaux lézard spock"/>
-    <s v="Pierre_papier_ciseaux_lezard_spock.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Sheldon est là"/>
-    <s v="Sheldon_est_la.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Sheldon raconte son rêve avec Spoke"/>
-    <s v="Sheldon_raconte_son_reve_avec_Spoke.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Theme full"/>
+    <s v="TBBT_Theme_full.mp3"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Bongo Song"/>
+    <s v="ZAZZ_Bongo_Song.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Brave Leonard song"/>
+    <s v="ZAZZ_Brave_Leonard_song.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="DNA of leonard nimoy"/>
+    <s v="ZAZZ_DNA_of_leonard_nimoy.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Dr Sheldon Cooper FTW"/>
+    <s v="ZAZZ_Dr_Sheldon_Cooper_FTW.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Engineering oompa loompas"/>
+    <s v="ZAZZ_Engineering_oompa_loompas.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Forgot Flash Drive"/>
+    <s v="forgot_flash_drive.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Goodnight puny human"/>
+    <s v="en_goodnight_puny_human.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="It's a trap!"/>
+    <s v="ZAZZ_It's_a_trap1.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="My brain is better than EVERYBODY'S! "/>
+    <s v="brain_better_than_everybody.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="My precious"/>
+    <s v="en_precious.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Penny Blossom Song"/>
+    <s v="ZAZZ_Penny_Blossom_Song.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Sheldon sings drunk"/>
+    <s v="ZAZZ_Sheldon_drunk_sings.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Soft Kitty"/>
+    <s v="ZAZZ_Sheldon_soft_kitty.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Suffer in silence"/>
+    <s v="suffer_in_silence.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="To Sheldon live long and prosper"/>
+    <s v="ZAZZ_To_Sheldon_live_long_and_prosper.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="we're taking the train"/>
+    <s v="ZAZZ_we're_taking_the_train.mp3"/>
+    <x v="2"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="Wheaton Wheaton Wheaton!"/>
     <s v="wheaton.mp3"/>
     <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Whip! Eh-hee"/>
-    <s v="Whip_eh_hee.mp3"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Bazinga one of my jokes"/>
-    <s v="CLAS_bazinga_one_of_my_jokes.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Bazinga!"/>
-    <s v="CLAS_Bazinga1.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Change is never fine"/>
-    <s v="CLAS_change_is_never_fine.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Hello honeypuffs"/>
-    <s v="CLAS_hello_honeypuffs.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="I'm Batman"/>
-    <s v="en_Im_Batman.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="It's not bad it's horrible"/>
-    <s v="CLAS_not_bad_it_s_horrible.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Knock knock knock Penny"/>
-    <s v="CLAS_knock_knock_knock_Penny.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Mua ah ah"/>
-    <s v="CLAS_mua_ah_ah.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Ooohu"/>
-    <s v="CLAS_oouh.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="peace out"/>
-    <s v="CLAS_peace_out.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Rock Paper Scissor Lizard Spock"/>
-    <s v="CLAS_Rock_Paper_Scissor_Lizard_Spock.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Sheldon laugh"/>
-    <s v="CLAS_Sheldon_laugh.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="There there"/>
-    <s v="CLAS_there_there.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="You're in my spot"/>
-    <s v="CLAS_You're_in_my_spot.mp3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Theme full"/>
-    <s v="TBBT_Theme_full.mp3"/>
-    <x v="1"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Theme end"/>
-    <s v="TBBT_Theme_end.mp3"/>
-    <x v="1"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Bongo Song"/>
-    <s v="ZAZZ_Bongo_Song.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Brave Leonard song"/>
-    <s v="ZAZZ_Brave_Leonard_song.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="DNA of leonard nimoy"/>
-    <s v="ZAZZ_DNA_of_leonard_nimoy.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Dr Sheldon Cooper FTW"/>
-    <s v="ZAZZ_Dr_Sheldon_Cooper_FTW.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Engineering oompa loompas"/>
-    <s v="ZAZZ_Engineering_oompa_loompas.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Goodnight puny human"/>
-    <s v="en_goodnight_puny_human.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="It's a trap!"/>
-    <s v="ZAZZ_It's_a_trap1.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="My precious"/>
-    <s v="en_precious.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Penny Blossom Song"/>
-    <s v="ZAZZ_Penny_Blossom_Song.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Sheldon sings drunk"/>
-    <s v="ZAZZ_Sheldon_drunk_sings.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Soft Kitty"/>
-    <s v="ZAZZ_Sheldon_soft_kitty.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Suffer in silence"/>
-    <s v="suffer_in_silence.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="To Sheldon live long and prosper"/>
-    <s v="ZAZZ_To_Sheldon_live_long_and_prosper.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="we're taking the train"/>
-    <s v="ZAZZ_we're_taking_the_train.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Wheaton Wheaton Wheaton!"/>
-    <s v="wheaton.mp3"/>
-    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
@@ -1857,12 +1873,6 @@
   <r>
     <s v="WoW Hacking"/>
     <s v="ZAZZ_WoW_Hacking.mp3"/>
-    <x v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="Forgot Flash Drive"/>
-    <s v="forgot_flash_drive.mp3"/>
     <x v="2"/>
     <x v="1"/>
   </r>
@@ -1870,7 +1880,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A10:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -1911,7 +1921,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -2012,9 +2022,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:D67" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:D67"/>
-  <sortState ref="A2:D67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:D68" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:D68"/>
+  <sortState ref="A2:D68">
     <sortCondition descending="1" ref="D2:D66"/>
     <sortCondition ref="C2:C66"/>
     <sortCondition ref="A2:A66"/>
@@ -2300,21 +2310,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" customWidth="1"/>
+    <col min="1" max="1" width="46.453125" customWidth="1"/>
     <col min="2" max="2" width="57" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2328,7 +2338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -2342,7 +2352,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2356,7 +2366,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -2370,7 +2380,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -2384,7 +2394,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -2398,7 +2408,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -2412,7 +2422,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -2426,7 +2436,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2440,7 +2450,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -2454,7 +2464,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -2468,12 +2478,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>36</v>
@@ -2482,12 +2492,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
         <v>36</v>
@@ -2496,7 +2506,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -2510,7 +2520,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -2524,7 +2534,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -2538,7 +2548,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2552,7 +2562,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
@@ -2566,7 +2576,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2580,7 +2590,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -2594,7 +2604,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -2608,7 +2618,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -2622,7 +2632,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>83</v>
       </c>
@@ -2636,7 +2646,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2650,7 +2660,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>85</v>
       </c>
@@ -2664,7 +2674,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -2678,7 +2688,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2692,7 +2702,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -2706,7 +2716,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -2720,7 +2730,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -2734,12 +2744,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -2748,9 +2758,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B32" t="s">
         <v>113</v>
@@ -2762,7 +2772,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -2776,7 +2786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -2790,7 +2800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -2804,7 +2814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -2818,7 +2828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>119</v>
       </c>
@@ -2832,7 +2842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -2846,7 +2856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -2860,7 +2870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>122</v>
       </c>
@@ -2874,7 +2884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -2888,7 +2898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -2902,7 +2912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -2916,7 +2926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -2930,9 +2940,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
         <v>17</v>
@@ -2944,7 +2954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -2958,12 +2968,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C47" t="s">
         <v>36</v>
@@ -2972,12 +2982,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C48" t="s">
         <v>36</v>
@@ -2986,7 +2996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -3000,7 +3010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -3014,7 +3024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -3028,7 +3038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>64</v>
       </c>
@@ -3042,7 +3052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -3056,13 +3066,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54" t="s">
         <v>136</v>
       </c>
-      <c r="B54" t="s">
-        <v>137</v>
-      </c>
       <c r="C54" t="s">
         <v>4</v>
       </c>
@@ -3070,12 +3080,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>4</v>
@@ -3084,7 +3094,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>72</v>
       </c>
@@ -3098,157 +3108,171 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>117</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>118</v>
       </c>
-      <c r="C57" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>66</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>28</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="C59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>79</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="C60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>78</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>30</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="C61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>132</v>
+      </c>
+      <c r="B62" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" t="s">
         <v>133</v>
       </c>
-      <c r="B61" t="s">
-        <v>132</v>
-      </c>
-      <c r="C61" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>67</v>
-      </c>
-      <c r="B62" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>68</v>
-      </c>
-      <c r="B63" t="s">
-        <v>32</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>129</v>
-      </c>
-      <c r="B64" t="s">
-        <v>128</v>
-      </c>
-      <c r="C64" t="s">
-        <v>4</v>
-      </c>
-      <c r="D64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>135</v>
-      </c>
-      <c r="B65" t="s">
-        <v>134</v>
-      </c>
-      <c r="C65" t="s">
-        <v>4</v>
-      </c>
-      <c r="D65" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>69</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>33</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="C67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>70</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>34</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D67" s="1" t="s">
+      <c r="C68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3265,16 +3289,16 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -3282,15 +3306,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" t="s">
         <v>123</v>
       </c>
-      <c r="B3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>37</v>
       </c>
@@ -3298,7 +3322,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
@@ -3306,31 +3330,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>35</v>
       </c>

</xml_diff>